<commit_message>
The SOR based on greedy algorithm
</commit_message>
<xml_diff>
--- a/data/orders.xlsx
+++ b/data/orders.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\course\project\SOR\code\Smart-Order-Router\Executor\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\course\project\SOR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E84404D-0422-4D8F-A3F7-4A8824C20385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A4DFA5-2956-443A-9FC9-B774A408D04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="19200" windowHeight="11170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microsofts" sheetId="1" r:id="rId1"/>
@@ -992,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="A1:D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1039,7 +1039,7 @@
         <v>200</v>
       </c>
       <c r="C4">
-        <v>183.92</v>
+        <v>183.97</v>
       </c>
       <c r="D4">
         <v>300</v>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>183.62</v>
+        <v>183.92</v>
       </c>
       <c r="B6">
         <v>1450</v>
@@ -1075,13 +1075,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>183.61</v>
+        <v>183.81</v>
       </c>
       <c r="B7">
         <v>1000</v>
       </c>
       <c r="C7">
-        <v>183.95</v>
+        <v>183.85</v>
       </c>
       <c r="D7">
         <v>200</v>
@@ -1136,7 +1136,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>183.63</v>
+        <v>183.73</v>
       </c>
       <c r="B12">
         <v>175</v>
@@ -1164,13 +1164,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>183.61</v>
+        <v>183.71</v>
       </c>
       <c r="B14">
         <v>1050</v>
       </c>
       <c r="C14">
-        <v>183.98</v>
+        <v>183.78</v>
       </c>
       <c r="D14">
         <v>180</v>
@@ -1186,7 +1186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8294AB8-021B-4FF9-A56B-246DE0BF2909}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>